<commit_message>
add Telmen of Mongolia to ps file
</commit_message>
<xml_diff>
--- a/气象/站点信息.xlsx
+++ b/气象/站点信息.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\文档\GIT SYNC\default\气象\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC24507-7362-4185-8420-4A7D9D16E2C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{113C120F-5D93-48FC-9338-E1B9B45D1932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{844553AA-A2A2-41AF-B6A7-7782726BF58F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="565">
   <si>
     <t>USAF</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2777,7 +2777,7 @@
   <dimension ref="A1:V154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -3050,32 +3050,30 @@
       <c r="J5" s="8"/>
       <c r="K5" s="7"/>
       <c r="L5" s="11">
-        <v>274</v>
-      </c>
-      <c r="M5" s="17">
-        <v>47.209609999999998</v>
-      </c>
-      <c r="N5" s="17">
-        <v>97.604699999999994</v>
+        <v>686</v>
+      </c>
+      <c r="M5" s="18">
+        <v>48.646230555555498</v>
+      </c>
+      <c r="N5" s="18">
+        <v>97.612224999999995</v>
       </c>
       <c r="O5" s="33">
-        <v>2156</v>
+        <v>1811</v>
       </c>
       <c r="P5" s="20" t="s">
-        <v>228</v>
+        <v>328</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="S5" s="10"/>
       <c r="T5" s="7"/>
       <c r="U5" s="11"/>
-      <c r="V5" s="7" t="s">
-        <v>537</v>
-      </c>
+      <c r="V5" s="7"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
@@ -3094,7 +3092,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
@@ -3102,30 +3100,32 @@
       <c r="J6" s="8"/>
       <c r="K6" s="7"/>
       <c r="L6" s="11">
-        <v>893</v>
-      </c>
-      <c r="M6" s="18">
-        <v>51.356372219999997</v>
-      </c>
-      <c r="N6" s="18">
-        <v>99.344038889999993</v>
+        <v>274</v>
+      </c>
+      <c r="M6" s="17">
+        <v>47.209609999999998</v>
+      </c>
+      <c r="N6" s="17">
+        <v>97.604699999999994</v>
       </c>
       <c r="O6" s="33">
-        <v>1546</v>
+        <v>2156</v>
       </c>
       <c r="P6" s="20" t="s">
-        <v>385</v>
+        <v>228</v>
       </c>
       <c r="Q6" s="9" t="s">
         <v>389</v>
       </c>
       <c r="R6" s="7" t="s">
-        <v>516</v>
+        <v>271</v>
       </c>
       <c r="S6" s="10"/>
       <c r="T6" s="7"/>
       <c r="U6" s="11"/>
-      <c r="V6" s="7"/>
+      <c r="V6" s="7" t="s">
+        <v>537</v>
+      </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A7" s="7" t="s">
@@ -3144,7 +3144,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -3152,25 +3152,25 @@
       <c r="J7" s="8"/>
       <c r="K7" s="7"/>
       <c r="L7" s="11">
-        <v>243</v>
-      </c>
-      <c r="M7" s="17">
-        <v>49.748916600000001</v>
-      </c>
-      <c r="N7" s="17">
-        <v>106.661469</v>
+        <v>893</v>
+      </c>
+      <c r="M7" s="18">
+        <v>51.356372219999997</v>
+      </c>
+      <c r="N7" s="18">
+        <v>99.344038889999993</v>
       </c>
       <c r="O7" s="33">
-        <v>675</v>
+        <v>1546</v>
       </c>
       <c r="P7" s="20" t="s">
-        <v>227</v>
+        <v>385</v>
       </c>
       <c r="Q7" s="9" t="s">
         <v>389</v>
       </c>
       <c r="R7" s="7" t="s">
-        <v>272</v>
+        <v>516</v>
       </c>
       <c r="S7" s="10"/>
       <c r="T7" s="7"/>
@@ -3194,46 +3194,40 @@
         <v>0</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="8">
-        <v>44212</v>
-      </c>
-      <c r="K8" s="7">
-        <v>99999</v>
-      </c>
-      <c r="L8" s="11"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="11">
+        <v>243</v>
+      </c>
       <c r="M8" s="17">
-        <v>49.971620000000001</v>
+        <v>49.748916600000001</v>
       </c>
       <c r="N8" s="17">
-        <v>92.077960000000004</v>
+        <v>106.661469</v>
       </c>
       <c r="O8" s="33">
-        <v>937</v>
+        <v>675</v>
       </c>
       <c r="P8" s="20" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="Q8" s="9" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="R8" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="S8" s="10" t="s">
-        <v>387</v>
-      </c>
-      <c r="T8" s="7" t="s">
-        <v>395</v>
-      </c>
+        <v>272</v>
+      </c>
+      <c r="S8" s="10"/>
+      <c r="T8" s="7"/>
       <c r="U8" s="11"/>
       <c r="V8" s="7"/>
     </row>
-    <row r="9" spans="1:22" ht="27.75" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
         <v>262</v>
       </c>
@@ -3250,46 +3244,44 @@
         <v>0</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="8">
-        <v>44221</v>
+        <v>44212</v>
       </c>
       <c r="K9" s="7">
         <v>99999</v>
       </c>
       <c r="L9" s="11"/>
       <c r="M9" s="17">
-        <v>49.700499999999998</v>
+        <v>49.971620000000001</v>
       </c>
       <c r="N9" s="17">
-        <v>96.363399999999999</v>
+        <v>92.077960000000004</v>
       </c>
       <c r="O9" s="33">
-        <v>1424</v>
+        <v>937</v>
       </c>
       <c r="P9" s="20" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="Q9" s="9" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="R9" s="7" t="s">
-        <v>269</v>
+        <v>515</v>
       </c>
       <c r="S9" s="10" t="s">
         <v>387</v>
       </c>
       <c r="T9" s="7" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="U9" s="11"/>
-      <c r="V9" s="7" t="s">
-        <v>540</v>
-      </c>
+      <c r="V9" s="7"/>
     </row>
     <row r="10" spans="1:22" ht="27.75" x14ac:dyDescent="0.4">
       <c r="A10" s="7" t="s">
@@ -3314,42 +3306,42 @@
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
       <c r="J10" s="8">
-        <v>44224</v>
+        <v>44221</v>
       </c>
       <c r="K10" s="7">
         <v>99999</v>
       </c>
       <c r="L10" s="11"/>
       <c r="M10" s="17">
-        <v>48.747999999999998</v>
+        <v>49.700499999999998</v>
       </c>
       <c r="N10" s="17">
-        <v>96.004249999999999</v>
+        <v>96.363399999999999</v>
       </c>
       <c r="O10" s="33">
-        <v>1931</v>
+        <v>1424</v>
       </c>
       <c r="P10" s="20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="Q10" s="9" t="s">
         <v>389</v>
       </c>
       <c r="R10" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="S10" s="10" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="T10" s="7" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="U10" s="11"/>
       <c r="V10" s="7" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.4">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="27.75" x14ac:dyDescent="0.4">
       <c r="A11" s="7" t="s">
         <v>262</v>
       </c>
@@ -3372,38 +3364,40 @@
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="8">
-        <v>44225</v>
+        <v>44224</v>
       </c>
       <c r="K11" s="7">
         <v>99999</v>
       </c>
       <c r="L11" s="11"/>
       <c r="M11" s="17">
-        <v>48.763053900000003</v>
+        <v>48.747999999999998</v>
       </c>
       <c r="N11" s="17">
-        <v>98.266199999999998</v>
+        <v>96.004249999999999</v>
       </c>
       <c r="O11" s="33">
-        <v>1726</v>
+        <v>1931</v>
       </c>
       <c r="P11" s="20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Q11" s="9" t="s">
         <v>389</v>
       </c>
       <c r="R11" s="7" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="S11" s="10" t="s">
         <v>386</v>
       </c>
       <c r="T11" s="7" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="U11" s="11"/>
-      <c r="V11" s="7"/>
+      <c r="V11" s="7" t="s">
+        <v>541</v>
+      </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A12" s="7" t="s">
@@ -3422,41 +3416,41 @@
         <v>0</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
       <c r="J12" s="8">
-        <v>44203</v>
+        <v>44225</v>
       </c>
       <c r="K12" s="7">
         <v>99999</v>
       </c>
       <c r="L12" s="11"/>
       <c r="M12" s="17">
-        <v>51.113950000000003</v>
+        <v>48.763053900000003</v>
       </c>
       <c r="N12" s="17">
-        <v>99.668563800000001</v>
+        <v>98.266199999999998</v>
       </c>
       <c r="O12" s="33">
-        <v>1585</v>
+        <v>1726</v>
       </c>
       <c r="P12" s="20" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="Q12" s="9" t="s">
         <v>389</v>
       </c>
       <c r="R12" s="7" t="s">
-        <v>516</v>
+        <v>273</v>
       </c>
       <c r="S12" s="10" t="s">
         <v>386</v>
       </c>
       <c r="T12" s="7" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="U12" s="11"/>
       <c r="V12" s="7"/>
@@ -3478,46 +3472,46 @@
         <v>0</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
       <c r="J13" s="8">
-        <v>44292</v>
+        <v>44203</v>
       </c>
       <c r="K13" s="7">
         <v>99999</v>
       </c>
       <c r="L13" s="11"/>
       <c r="M13" s="17">
-        <v>47.918445599999998</v>
+        <v>51.113950000000003</v>
       </c>
       <c r="N13" s="17">
-        <v>106.848343</v>
+        <v>99.668563800000001</v>
       </c>
       <c r="O13" s="33">
-        <v>1304</v>
+        <v>1585</v>
       </c>
       <c r="P13" s="20" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="Q13" s="9" t="s">
         <v>389</v>
       </c>
       <c r="R13" s="7" t="s">
-        <v>272</v>
+        <v>516</v>
       </c>
       <c r="S13" s="10" t="s">
         <v>386</v>
       </c>
       <c r="T13" s="7" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="U13" s="11"/>
       <c r="V13" s="7"/>
     </row>
-    <row r="14" spans="1:22" ht="27.75" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A14" s="7" t="s">
         <v>262</v>
       </c>
@@ -3530,44 +3524,52 @@
       <c r="D14" s="25">
         <v>13</v>
       </c>
-      <c r="E14" s="28"/>
+      <c r="E14" s="28">
+        <v>0</v>
+      </c>
       <c r="F14" s="7" t="s">
-        <v>535</v>
+        <v>261</v>
       </c>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="11">
-        <v>546</v>
-      </c>
-      <c r="M14" s="18">
-        <v>47.227308333333298</v>
-      </c>
-      <c r="N14" s="18">
-        <v>98.573644444444398</v>
+      <c r="J14" s="8">
+        <v>44292</v>
+      </c>
+      <c r="K14" s="7">
+        <v>99999</v>
+      </c>
+      <c r="L14" s="11"/>
+      <c r="M14" s="17">
+        <v>47.918445599999998</v>
+      </c>
+      <c r="N14" s="17">
+        <v>106.848343</v>
       </c>
       <c r="O14" s="33">
-        <v>2422</v>
+        <v>1304</v>
       </c>
       <c r="P14" s="20" t="s">
-        <v>363</v>
-      </c>
-      <c r="Q14" s="9"/>
+        <v>247</v>
+      </c>
+      <c r="Q14" s="9" t="s">
+        <v>389</v>
+      </c>
       <c r="R14" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="S14" s="10"/>
-      <c r="T14" s="7"/>
+        <v>272</v>
+      </c>
+      <c r="S14" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="T14" s="7" t="s">
+        <v>400</v>
+      </c>
       <c r="U14" s="11"/>
-      <c r="V14" s="7" t="s">
-        <v>542</v>
-      </c>
+      <c r="V14" s="7"/>
     </row>
     <row r="15" spans="1:22" ht="27.75" x14ac:dyDescent="0.4">
       <c r="A15" s="7" t="s">
-        <v>347</v>
+        <v>262</v>
       </c>
       <c r="B15" s="22" t="s">
         <v>391</v>
@@ -3588,19 +3590,19 @@
       <c r="J15" s="8"/>
       <c r="K15" s="7"/>
       <c r="L15" s="11">
-        <v>276</v>
-      </c>
-      <c r="M15" s="17">
-        <v>47.016469999999998</v>
-      </c>
-      <c r="N15" s="17">
-        <v>99.479550000000003</v>
+        <v>546</v>
+      </c>
+      <c r="M15" s="18">
+        <v>47.227308333333298</v>
+      </c>
+      <c r="N15" s="18">
+        <v>98.573644444444398</v>
       </c>
       <c r="O15" s="33">
-        <v>2034</v>
+        <v>2422</v>
       </c>
       <c r="P15" s="20" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="Q15" s="9"/>
       <c r="R15" s="7" t="s">
@@ -3609,11 +3611,13 @@
       <c r="S15" s="10"/>
       <c r="T15" s="7"/>
       <c r="U15" s="11"/>
-      <c r="V15" s="7"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="V15" s="7" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="27.75" x14ac:dyDescent="0.4">
       <c r="A16" s="7" t="s">
-        <v>262</v>
+        <v>347</v>
       </c>
       <c r="B16" s="22" t="s">
         <v>391</v>
@@ -3626,7 +3630,7 @@
       </c>
       <c r="E16" s="28"/>
       <c r="F16" s="7" t="s">
-        <v>330</v>
+        <v>535</v>
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
@@ -3634,23 +3638,23 @@
       <c r="J16" s="8"/>
       <c r="K16" s="7"/>
       <c r="L16" s="11">
-        <v>864</v>
+        <v>276</v>
       </c>
       <c r="M16" s="17">
-        <v>48.332500000000003</v>
+        <v>47.016469999999998</v>
       </c>
       <c r="N16" s="17">
-        <v>92.634159999999994</v>
+        <v>99.479550000000003</v>
       </c>
       <c r="O16" s="33">
-        <v>1166</v>
+        <v>2034</v>
       </c>
       <c r="P16" s="20" t="s">
-        <v>339</v>
+        <v>364</v>
       </c>
       <c r="Q16" s="9"/>
       <c r="R16" s="7" t="s">
-        <v>357</v>
+        <v>270</v>
       </c>
       <c r="S16" s="10"/>
       <c r="T16" s="7"/>
@@ -3680,19 +3684,19 @@
       <c r="J17" s="8"/>
       <c r="K17" s="7"/>
       <c r="L17" s="11">
-        <v>863</v>
-      </c>
-      <c r="M17" s="18">
-        <v>48.501372222222201</v>
-      </c>
-      <c r="N17" s="18">
-        <v>91.448158333333296</v>
+        <v>864</v>
+      </c>
+      <c r="M17" s="17">
+        <v>48.332500000000003</v>
+      </c>
+      <c r="N17" s="17">
+        <v>92.634159999999994</v>
       </c>
       <c r="O17" s="33">
-        <v>1262</v>
+        <v>1166</v>
       </c>
       <c r="P17" s="20" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="Q17" s="9"/>
       <c r="R17" s="7" t="s">
@@ -3726,23 +3730,23 @@
       <c r="J18" s="8"/>
       <c r="K18" s="7"/>
       <c r="L18" s="11">
-        <v>271</v>
-      </c>
-      <c r="M18" s="17">
-        <v>46.590800000000002</v>
-      </c>
-      <c r="N18" s="17">
-        <v>93.272199999999998</v>
+        <v>863</v>
+      </c>
+      <c r="M18" s="18">
+        <v>48.501372222222201</v>
+      </c>
+      <c r="N18" s="18">
+        <v>91.448158333333296</v>
       </c>
       <c r="O18" s="33">
-        <v>1716</v>
+        <v>1262</v>
       </c>
       <c r="P18" s="20" t="s">
-        <v>331</v>
+        <v>346</v>
       </c>
       <c r="Q18" s="9"/>
       <c r="R18" s="7" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="S18" s="10"/>
       <c r="T18" s="7"/>
@@ -3751,7 +3755,7 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A19" s="7" t="s">
-        <v>347</v>
+        <v>262</v>
       </c>
       <c r="B19" s="22" t="s">
         <v>391</v>
@@ -3764,7 +3768,7 @@
       </c>
       <c r="E19" s="28"/>
       <c r="F19" s="7" t="s">
-        <v>348</v>
+        <v>330</v>
       </c>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
@@ -3772,22 +3776,24 @@
       <c r="J19" s="8"/>
       <c r="K19" s="7"/>
       <c r="L19" s="11">
-        <v>889</v>
-      </c>
-      <c r="M19" s="18">
-        <v>49.597225000000002</v>
-      </c>
-      <c r="N19" s="18">
-        <v>98.695800000000006</v>
+        <v>271</v>
+      </c>
+      <c r="M19" s="17">
+        <v>46.590800000000002</v>
+      </c>
+      <c r="N19" s="17">
+        <v>93.272199999999998</v>
       </c>
       <c r="O19" s="33">
-        <v>1805</v>
+        <v>1716</v>
       </c>
       <c r="P19" s="20" t="s">
-        <v>349</v>
+        <v>331</v>
       </c>
       <c r="Q19" s="9"/>
-      <c r="R19" s="7"/>
+      <c r="R19" s="7" t="s">
+        <v>355</v>
+      </c>
       <c r="S19" s="10"/>
       <c r="T19" s="7"/>
       <c r="U19" s="11"/>
@@ -3816,24 +3822,22 @@
       <c r="J20" s="8"/>
       <c r="K20" s="7"/>
       <c r="L20" s="11">
-        <v>887</v>
+        <v>889</v>
       </c>
       <c r="M20" s="18">
-        <v>50.677022222222199</v>
+        <v>49.597225000000002</v>
       </c>
       <c r="N20" s="18">
-        <v>99.226799999999997</v>
+        <v>98.695800000000006</v>
       </c>
       <c r="O20" s="33">
-        <v>1687</v>
+        <v>1805</v>
       </c>
       <c r="P20" s="20" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="Q20" s="9"/>
-      <c r="R20" s="7" t="s">
-        <v>516</v>
-      </c>
+      <c r="R20" s="7"/>
       <c r="S20" s="10"/>
       <c r="T20" s="7"/>
       <c r="U20" s="11"/>
@@ -3854,7 +3858,7 @@
       </c>
       <c r="E21" s="28"/>
       <c r="F21" s="7" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
@@ -3862,23 +3866,23 @@
       <c r="J21" s="8"/>
       <c r="K21" s="7"/>
       <c r="L21" s="11">
-        <v>774</v>
+        <v>887</v>
       </c>
       <c r="M21" s="18">
-        <v>50.069886111111103</v>
+        <v>50.677022222222199</v>
       </c>
       <c r="N21" s="18">
-        <v>105.884363888888</v>
+        <v>99.226799999999997</v>
       </c>
       <c r="O21" s="33">
-        <v>632</v>
+        <v>1687</v>
       </c>
       <c r="P21" s="20" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="Q21" s="9"/>
       <c r="R21" s="7" t="s">
-        <v>352</v>
+        <v>516</v>
       </c>
       <c r="S21" s="10"/>
       <c r="T21" s="7"/>
@@ -3887,7 +3891,7 @@
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A22" s="7" t="s">
-        <v>262</v>
+        <v>347</v>
       </c>
       <c r="B22" s="22" t="s">
         <v>391</v>
@@ -3900,7 +3904,7 @@
       </c>
       <c r="E22" s="28"/>
       <c r="F22" s="7" t="s">
-        <v>249</v>
+        <v>350</v>
       </c>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
@@ -3908,23 +3912,23 @@
       <c r="J22" s="8"/>
       <c r="K22" s="7"/>
       <c r="L22" s="11">
-        <v>827</v>
+        <v>774</v>
       </c>
       <c r="M22" s="18">
-        <v>50.610586111111097</v>
+        <v>50.069886111111103</v>
       </c>
       <c r="N22" s="18">
-        <v>92.402124999999998</v>
+        <v>105.884363888888</v>
       </c>
       <c r="O22" s="33">
-        <v>859</v>
+        <v>632</v>
       </c>
       <c r="P22" s="20" t="s">
-        <v>338</v>
+        <v>351</v>
       </c>
       <c r="Q22" s="9"/>
       <c r="R22" s="7" t="s">
-        <v>517</v>
+        <v>352</v>
       </c>
       <c r="S22" s="10"/>
       <c r="T22" s="7"/>
@@ -3954,23 +3958,23 @@
       <c r="J23" s="8"/>
       <c r="K23" s="7"/>
       <c r="L23" s="11">
-        <v>201</v>
-      </c>
-      <c r="M23" s="17">
-        <v>49.72889</v>
-      </c>
-      <c r="N23" s="17">
-        <v>93.268609999999995</v>
+        <v>827</v>
+      </c>
+      <c r="M23" s="18">
+        <v>50.610586111111097</v>
+      </c>
+      <c r="N23" s="18">
+        <v>92.402124999999998</v>
       </c>
       <c r="O23" s="33">
-        <v>1393</v>
+        <v>859</v>
       </c>
       <c r="P23" s="20" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="Q23" s="9"/>
       <c r="R23" s="7" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="S23" s="10"/>
       <c r="T23" s="7"/>
@@ -3979,7 +3983,7 @@
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A24" s="7" t="s">
-        <v>347</v>
+        <v>262</v>
       </c>
       <c r="B24" s="22" t="s">
         <v>391</v>
@@ -3992,7 +3996,7 @@
       </c>
       <c r="E24" s="28"/>
       <c r="F24" s="7" t="s">
-        <v>360</v>
+        <v>249</v>
       </c>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
@@ -4000,23 +4004,23 @@
       <c r="J24" s="8"/>
       <c r="K24" s="7"/>
       <c r="L24" s="11">
-        <v>215</v>
-      </c>
-      <c r="M24" s="18">
-        <v>49.104990000000001</v>
-      </c>
-      <c r="N24" s="18">
-        <v>91.726190000000003</v>
+        <v>201</v>
+      </c>
+      <c r="M24" s="17">
+        <v>49.72889</v>
+      </c>
+      <c r="N24" s="17">
+        <v>93.268609999999995</v>
       </c>
       <c r="O24" s="33">
-        <v>1593</v>
+        <v>1393</v>
       </c>
       <c r="P24" s="20" t="s">
-        <v>361</v>
+        <v>329</v>
       </c>
       <c r="Q24" s="9"/>
       <c r="R24" s="7" t="s">
-        <v>362</v>
+        <v>515</v>
       </c>
       <c r="S24" s="10"/>
       <c r="T24" s="7"/>
@@ -4025,7 +4029,7 @@
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A25" s="7" t="s">
-        <v>262</v>
+        <v>347</v>
       </c>
       <c r="B25" s="22" t="s">
         <v>391</v>
@@ -4038,7 +4042,7 @@
       </c>
       <c r="E25" s="28"/>
       <c r="F25" s="7" t="s">
-        <v>249</v>
+        <v>360</v>
       </c>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
@@ -4046,23 +4050,23 @@
       <c r="J25" s="8"/>
       <c r="K25" s="7"/>
       <c r="L25" s="11">
-        <v>834</v>
+        <v>215</v>
       </c>
       <c r="M25" s="18">
-        <v>50.339719444444398</v>
+        <v>49.104990000000001</v>
       </c>
       <c r="N25" s="18">
-        <v>91.604813888888799</v>
+        <v>91.726190000000003</v>
       </c>
       <c r="O25" s="33">
-        <v>1142</v>
+        <v>1593</v>
       </c>
       <c r="P25" s="20" t="s">
-        <v>336</v>
+        <v>361</v>
       </c>
       <c r="Q25" s="9"/>
       <c r="R25" s="7" t="s">
-        <v>517</v>
+        <v>362</v>
       </c>
       <c r="S25" s="10"/>
       <c r="T25" s="7"/>
@@ -4092,23 +4096,23 @@
       <c r="J26" s="8"/>
       <c r="K26" s="7"/>
       <c r="L26" s="11">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="M26" s="18">
-        <v>50.097880555555498</v>
+        <v>50.339719444444398</v>
       </c>
       <c r="N26" s="18">
-        <v>91.676269444444401</v>
+        <v>91.604813888888799</v>
       </c>
       <c r="O26" s="33">
-        <v>1212</v>
+        <v>1142</v>
       </c>
       <c r="P26" s="20" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="Q26" s="9"/>
       <c r="R26" s="7" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="S26" s="10"/>
       <c r="T26" s="7"/>
@@ -4135,30 +4139,26 @@
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
-      <c r="J27" s="8">
-        <v>44213</v>
-      </c>
-      <c r="K27" s="7">
-        <v>99999</v>
-      </c>
+      <c r="J27" s="8"/>
+      <c r="K27" s="7"/>
       <c r="L27" s="11">
-        <v>213</v>
-      </c>
-      <c r="M27" s="17">
-        <v>49.658639999999998</v>
-      </c>
-      <c r="N27" s="17">
-        <v>94.404060000000001</v>
+        <v>836</v>
+      </c>
+      <c r="M27" s="18">
+        <v>50.097880555555498</v>
+      </c>
+      <c r="N27" s="18">
+        <v>91.676269444444401</v>
       </c>
       <c r="O27" s="33">
-        <v>1233</v>
+        <v>1212</v>
       </c>
       <c r="P27" s="20" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="Q27" s="9"/>
       <c r="R27" s="7" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="S27" s="10"/>
       <c r="T27" s="7"/>
@@ -4185,26 +4185,30 @@
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="7"/>
+      <c r="J28" s="8">
+        <v>44213</v>
+      </c>
+      <c r="K28" s="7">
+        <v>99999</v>
+      </c>
       <c r="L28" s="11">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="M28" s="17">
-        <v>48.821666700000002</v>
+        <v>49.658639999999998</v>
       </c>
       <c r="N28" s="17">
-        <v>93.103059999999999</v>
+        <v>94.404060000000001</v>
       </c>
       <c r="O28" s="33">
-        <v>1045</v>
+        <v>1233</v>
       </c>
       <c r="P28" s="20" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="Q28" s="9"/>
       <c r="R28" s="7" t="s">
-        <v>354</v>
+        <v>515</v>
       </c>
       <c r="S28" s="10"/>
       <c r="T28" s="7"/>
@@ -4226,7 +4230,7 @@
       </c>
       <c r="E29" s="28"/>
       <c r="F29" s="7" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
@@ -4234,23 +4238,23 @@
       <c r="J29" s="8"/>
       <c r="K29" s="7"/>
       <c r="L29" s="11">
-        <v>677</v>
-      </c>
-      <c r="M29" s="18">
-        <v>49.373166666666599</v>
-      </c>
-      <c r="N29" s="18">
-        <v>96.414816666666596</v>
+        <v>216</v>
+      </c>
+      <c r="M29" s="17">
+        <v>48.821666700000002</v>
+      </c>
+      <c r="N29" s="17">
+        <v>93.103059999999999</v>
       </c>
       <c r="O29" s="33">
-        <v>1858</v>
+        <v>1045</v>
       </c>
       <c r="P29" s="20" t="s">
-        <v>344</v>
+        <v>327</v>
       </c>
       <c r="Q29" s="9"/>
       <c r="R29" s="7" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="S29" s="10"/>
       <c r="T29" s="7"/>
@@ -4280,23 +4284,23 @@
       <c r="J30" s="8"/>
       <c r="K30" s="7"/>
       <c r="L30" s="11">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="M30" s="18">
-        <v>48.721816666666598</v>
+        <v>49.373166666666599</v>
       </c>
       <c r="N30" s="18">
-        <v>98.794905555555502</v>
+        <v>96.414816666666596</v>
       </c>
       <c r="O30" s="33">
-        <v>1656</v>
+        <v>1858</v>
       </c>
       <c r="P30" s="20" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="Q30" s="9"/>
       <c r="R30" s="7" t="s">
-        <v>273</v>
+        <v>358</v>
       </c>
       <c r="S30" s="10"/>
       <c r="T30" s="7"/>
@@ -4326,23 +4330,23 @@
       <c r="J31" s="8"/>
       <c r="K31" s="7"/>
       <c r="L31" s="11">
-        <v>220</v>
-      </c>
-      <c r="M31" s="17">
-        <v>48.870530000000002</v>
-      </c>
-      <c r="N31" s="17">
-        <v>96.961585999999997</v>
+        <v>680</v>
+      </c>
+      <c r="M31" s="18">
+        <v>48.721816666666598</v>
+      </c>
+      <c r="N31" s="18">
+        <v>98.794905555555502</v>
       </c>
       <c r="O31" s="33">
-        <v>1851</v>
+        <v>1656</v>
       </c>
       <c r="P31" s="20" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="Q31" s="9"/>
       <c r="R31" s="7" t="s">
-        <v>359</v>
+        <v>273</v>
       </c>
       <c r="S31" s="10"/>
       <c r="T31" s="7"/>
@@ -4372,23 +4376,23 @@
       <c r="J32" s="8"/>
       <c r="K32" s="7"/>
       <c r="L32" s="11">
-        <v>683</v>
-      </c>
-      <c r="M32" s="18">
-        <v>48.589822222222203</v>
-      </c>
-      <c r="N32" s="18">
-        <v>95.435675000000003</v>
+        <v>220</v>
+      </c>
+      <c r="M32" s="17">
+        <v>48.870530000000002</v>
+      </c>
+      <c r="N32" s="17">
+        <v>96.961585999999997</v>
       </c>
       <c r="O32" s="33">
-        <v>1569</v>
+        <v>1851</v>
       </c>
       <c r="P32" s="20" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
       <c r="Q32" s="9"/>
       <c r="R32" s="7" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="S32" s="10"/>
       <c r="T32" s="7"/>
@@ -4418,25 +4422,23 @@
       <c r="J33" s="8"/>
       <c r="K33" s="7"/>
       <c r="L33" s="11">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="M33" s="18">
-        <v>48.646230555555498</v>
+        <v>48.589822222222203</v>
       </c>
       <c r="N33" s="18">
-        <v>97.612224999999995</v>
+        <v>95.435675000000003</v>
       </c>
       <c r="O33" s="33">
-        <v>1811</v>
+        <v>1569</v>
       </c>
       <c r="P33" s="20" t="s">
-        <v>328</v>
-      </c>
-      <c r="Q33" s="9" t="s">
-        <v>390</v>
-      </c>
+        <v>332</v>
+      </c>
+      <c r="Q33" s="9"/>
       <c r="R33" s="7" t="s">
-        <v>273</v>
+        <v>356</v>
       </c>
       <c r="S33" s="10"/>
       <c r="T33" s="7"/>
@@ -10718,7 +10720,7 @@
       <c r="V154" s="7"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="FV/KEXyogF1lqBtIZmjcYv1zCAUnNU3dWYWfm8CECdfhYydEK6O3qX4PBpDHXG2kKN7xPGBt0/xSzsuhwAN2dg==" saltValue="ZTR8kCezyUh5pFo/wIqxCQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="jOelCbdLCE3e0Kovt7EFVlM9TIOZJrhmI9XatRmdgfeBH+NBkq/2Eq6CxjuBaX/i3B54Nem/0KDfQWKcBaNhIg==" saltValue="WNMMOLo63AfzNKZ8b/4ElQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V141">
     <sortCondition ref="D2:D141"/>
     <sortCondition ref="B2:B141"/>
@@ -10728,7 +10730,7 @@
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A2:V154">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>IF(MOD(ROW(), 2), 0, 1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11569,7 +11571,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A2:V22">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>IF(MOD(ROW(), 2), 0, 1)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
move eastern siberia stations down to the bottom in excel
</commit_message>
<xml_diff>
--- a/气象/站点信息.xlsx
+++ b/气象/站点信息.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\文档\GIT SYNC\default\气象\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8982E237-6EA7-40D6-B448-206A3338EE71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E262D14-98A0-45C7-955A-84D804B3004F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{844553AA-A2A2-41AF-B6A7-7782726BF58F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1198" uniqueCount="565">
   <si>
     <t>USAF</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2777,7 +2777,7 @@
   <dimension ref="A1:V154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -7296,9 +7296,7 @@
       <c r="P85" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="Q85" s="9" t="s">
-        <v>389</v>
-      </c>
+      <c r="Q85" s="9"/>
       <c r="R85" s="7" t="s">
         <v>292</v>
       </c>
@@ -10720,7 +10718,7 @@
       <c r="V154" s="7"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="QxXSn38pjSVFSRBv4Ux07d6bk5IgUzTobhrNthUjK57SWYJwj93yH2V4wpuemQTC/kSW2Al1fl0U3UqBxHIkwQ==" saltValue="badUXvGNigBjrDUlO6uCQQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="+8uqFJVK6748xDKMq11nFoD7YY1ByTKqPRPEWNXVT6I40N9nSav0nIHARdLTSmHLmCQRStUVUniEDTqc/qXfTw==" saltValue="FY/QPsqHLYNmqS4KMCJLAw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V141">
     <sortCondition ref="D2:D141"/>
     <sortCondition ref="B2:B141"/>

</xml_diff>

<commit_message>
Add more Siberian Stations
</commit_message>
<xml_diff>
--- a/气象/站点信息.xlsx
+++ b/气象/站点信息.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\文档\GIT SYNC\default\气象\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DD4E43-0825-4607-AA75-AA240A7CC079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB9E239-B13A-4DD5-A9CC-5C249D8D23F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{844553AA-A2A2-41AF-B6A7-7782726BF58F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1218" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1242" uniqueCount="590">
   <si>
     <t>USAF</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2218,6 +2218,54 @@
   </si>
   <si>
     <t>俄罗斯后贝加尔边疆区【乌斯季卡连加】北纬54.45°，海拔686米。91-20十二月平均气温 -31.7℃，一月平均气温 -32.3℃，一月平均低温约-39.4℃，一月平均高温约-23.8℃，七月平均气温 17℃，年平均气温 -5.9℃。历史极端冷月均温 -40.0℃(1960-01)，极端低温 -56.9℃(1987-01-09)，极端高温 38.0℃(1976-07-17)，一月极端高温 -5.0℃(1958-01-04, 1974-01-02)，七月极端低温 -2.8℃(1987-07-01, 1990-07-24)。1986/1987冬至少有17天低温低于-50℃。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>楚科奇自治区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>奥莫隆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>奥莫隆河</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Omolon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>马加丹州</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Эльген</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>科雷马河</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taskan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>克拉斯诺亚尔斯克边疆区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tura</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图拉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通古斯卡河、坚边奇河</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2826,7 +2874,7 @@
   <dimension ref="A1:V156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -10572,75 +10620,165 @@
       <c r="U143" s="11"/>
       <c r="V143" s="7"/>
     </row>
-    <row r="144" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A144" s="14"/>
-      <c r="B144" s="22"/>
-      <c r="C144" s="22"/>
-      <c r="D144" s="25"/>
+    <row r="144" spans="1:22" ht="27.75" x14ac:dyDescent="0.4">
+      <c r="A144" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B144" s="22" t="s">
+        <v>480</v>
+      </c>
+      <c r="C144" s="22">
+        <v>11</v>
+      </c>
+      <c r="D144" s="25">
+        <v>143</v>
+      </c>
       <c r="E144" s="28"/>
-      <c r="F144" s="14"/>
+      <c r="F144" s="14" t="s">
+        <v>578</v>
+      </c>
       <c r="G144" s="14"/>
       <c r="H144" s="14"/>
       <c r="I144" s="14"/>
-      <c r="J144" s="8"/>
-      <c r="K144" s="14"/>
+      <c r="J144" s="8">
+        <v>25428</v>
+      </c>
+      <c r="K144" s="7">
+        <v>99999</v>
+      </c>
       <c r="L144" s="15"/>
-      <c r="M144" s="18"/>
-      <c r="N144" s="18"/>
-      <c r="O144" s="33"/>
-      <c r="P144" s="20"/>
-      <c r="Q144" s="9"/>
-      <c r="R144" s="14"/>
-      <c r="S144" s="10"/>
-      <c r="T144" s="14"/>
+      <c r="M144" s="18">
+        <v>65.233333299999998</v>
+      </c>
+      <c r="N144" s="18">
+        <v>160.53333330000001</v>
+      </c>
+      <c r="O144" s="33">
+        <v>264</v>
+      </c>
+      <c r="P144" s="20" t="s">
+        <v>579</v>
+      </c>
+      <c r="Q144" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="R144" s="14" t="s">
+        <v>580</v>
+      </c>
+      <c r="S144" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="T144" s="14" t="s">
+        <v>581</v>
+      </c>
       <c r="U144" s="11"/>
       <c r="V144" s="7"/>
     </row>
     <row r="145" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A145" s="14"/>
-      <c r="B145" s="22"/>
-      <c r="C145" s="22"/>
-      <c r="D145" s="25"/>
+      <c r="A145" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B145" s="22" t="s">
+        <v>480</v>
+      </c>
+      <c r="C145" s="22">
+        <v>12</v>
+      </c>
+      <c r="D145" s="25">
+        <v>144</v>
+      </c>
       <c r="E145" s="28"/>
-      <c r="F145" s="14"/>
+      <c r="F145" s="14" t="s">
+        <v>582</v>
+      </c>
       <c r="G145" s="14"/>
       <c r="H145" s="14"/>
       <c r="I145" s="14"/>
-      <c r="J145" s="8"/>
-      <c r="K145" s="14"/>
+      <c r="J145" s="8">
+        <v>25700</v>
+      </c>
+      <c r="K145" s="7">
+        <v>99999</v>
+      </c>
       <c r="L145" s="15"/>
-      <c r="M145" s="18"/>
-      <c r="N145" s="18"/>
-      <c r="O145" s="33"/>
-      <c r="P145" s="20"/>
-      <c r="Q145" s="9"/>
-      <c r="R145" s="14"/>
-      <c r="S145" s="10"/>
-      <c r="T145" s="14"/>
+      <c r="M145" s="18">
+        <v>62.8</v>
+      </c>
+      <c r="N145" s="18">
+        <v>150.66666660000001</v>
+      </c>
+      <c r="O145" s="33">
+        <v>312.39999999999998</v>
+      </c>
+      <c r="P145" s="20" t="s">
+        <v>583</v>
+      </c>
+      <c r="Q145" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="R145" s="14" t="s">
+        <v>584</v>
+      </c>
+      <c r="S145" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="T145" s="14" t="s">
+        <v>585</v>
+      </c>
       <c r="U145" s="11"/>
       <c r="V145" s="7"/>
     </row>
-    <row r="146" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A146" s="14"/>
-      <c r="B146" s="22"/>
-      <c r="C146" s="22"/>
-      <c r="D146" s="25"/>
+    <row r="146" spans="1:22" ht="41.65" x14ac:dyDescent="0.4">
+      <c r="A146" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B146" s="22" t="s">
+        <v>480</v>
+      </c>
+      <c r="C146" s="22">
+        <v>13</v>
+      </c>
+      <c r="D146" s="25">
+        <v>145</v>
+      </c>
       <c r="E146" s="28"/>
-      <c r="F146" s="14"/>
+      <c r="F146" s="14" t="s">
+        <v>586</v>
+      </c>
       <c r="G146" s="14"/>
       <c r="H146" s="14"/>
       <c r="I146" s="14"/>
-      <c r="J146" s="8"/>
-      <c r="K146" s="14"/>
+      <c r="J146" s="8">
+        <v>24507</v>
+      </c>
+      <c r="K146" s="7">
+        <v>99999</v>
+      </c>
       <c r="L146" s="15"/>
-      <c r="M146" s="18"/>
-      <c r="N146" s="18"/>
-      <c r="O146" s="33"/>
-      <c r="P146" s="20"/>
-      <c r="Q146" s="9"/>
-      <c r="R146" s="14"/>
-      <c r="S146" s="10"/>
-      <c r="T146" s="14"/>
+      <c r="M146" s="18">
+        <v>64.266666599999994</v>
+      </c>
+      <c r="N146" s="18">
+        <v>100.2333333</v>
+      </c>
+      <c r="O146" s="33">
+        <v>168</v>
+      </c>
+      <c r="P146" s="20" t="s">
+        <v>588</v>
+      </c>
+      <c r="Q146" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="R146" s="14" t="s">
+        <v>589</v>
+      </c>
+      <c r="S146" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="T146" s="14" t="s">
+        <v>587</v>
+      </c>
       <c r="U146" s="11"/>
       <c r="V146" s="7"/>
     </row>
@@ -10885,7 +11023,7 @@
       <c r="V156" s="7"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Yo3PYkQlboB6H2Zg7lgtVXtvzrMIe0d1m+4QVSfoBeORF4+OGeDnJQC6gvodgsdqHSEyDf70LcgOn/iaj2cJQA==" saltValue="mOCYM0lNYoqmbLlJQiiweg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="u4ZNA/OMijTgwwqAp43P95hS6RRdja6UqxUTjPKCw9BLXKb7g10fguLTEIm/7J+0dfHpqXfqO0ssJdgplOyz7g==" saltValue="pV3z+5COOglpGGckT53nWg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V143">
     <sortCondition ref="D2:D143"/>
     <sortCondition ref="B2:B143"/>

</xml_diff>